<commit_message>
add function: MACTH and INDEX
</commit_message>
<xml_diff>
--- a/excel/Examples.xlsx
+++ b/excel/Examples.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8921067-ECF9-4588-A9D0-051ADCB8B3C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2EADD5-54C5-451A-BF4A-FB1825D4C26E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>